<commit_message>
Changes in Mavlink wrapper Changes in plan text file Added sensor holder 3D model
</commit_message>
<xml_diff>
--- a/Documentos/Registro de gastos.xlsx
+++ b/Documentos/Registro de gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://continental-my.sharepoint.com/personal/uidd7372_contiwan_com/Documents/CCC/2022/3 - Custom Robotics/Talent Land/Hackathon/2023/Talent-Hackathon-2023/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC104847C19B7E105ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1779FECD-9096-4B94-938C-31CA545BD56E}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABDACC104847C19B7E105ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A30AE62-2257-4141-AD56-1C4B631FECC7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Descripción</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Pieza 3D</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +425,7 @@
       </c>
       <c r="D1" s="1">
         <f>SUM(B2:B49)</f>
-        <v>1684</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -479,6 +482,14 @@
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>